<commit_message>
Optimization 2 for MIP, settings.ini and contracts generation in Gen_contracts.ipynb
</commit_message>
<xml_diff>
--- a/RunTime_VS_Topology.xlsx
+++ b/RunTime_VS_Topology.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Изм.1" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Изм.2" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>Имя топологии</t>
   </si>
@@ -228,6 +229,123 @@
   </si>
   <si>
     <t>50.90</t>
+  </si>
+  <si>
+    <t>Количество неравенств</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21}]</t>
+  </si>
+  <si>
+    <t>1.79</t>
+  </si>
+  <si>
+    <t>4.27</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21},
+             {'volume': 200, 't_s':  10, 't':  50, 'A': 5, 'B': 26}]</t>
+  </si>
+  <si>
+    <t>4.29</t>
+  </si>
+  <si>
+    <t>5.14</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21},
+             {'volume': 200, 't_s':  10, 't':  50, 'A': 5, 'B': 26},
+             {'volume': 300, 't_s':  0, 't':  50, 'A': 4, 'B': 3}]</t>
+  </si>
+  <si>
+    <t>6.72</t>
+  </si>
+  <si>
+    <t>6.26</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21},
+             {'volume': 200, 't_s':  10, 't':  50, 'A': 5, 'B': 26},
+             {'volume': 300, 't_s':  0, 't':  50, 'A': 4, 'B': 3},
+             {'volume': 100, 't_s':  100, 't':  50, 'A': 9, 'B': 17}]</t>
+  </si>
+  <si>
+    <t>9.93</t>
+  </si>
+  <si>
+    <t>8.14</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21},
+             {'volume': 200, 't_s':  10, 't':  50, 'A': 5, 'B': 26},
+             {'volume': 300, 't_s':  0, 't':  50, 'A': 4, 'B': 3},
+             {'volume': 100, 't_s':  100, 't':  50, 'A': 9, 'B': 17},
+             {'volume': 200, 't_s':  0, 't':  20, 'A': 12, 'B': 19}]</t>
+  </si>
+  <si>
+    <t>10.99</t>
+  </si>
+  <si>
+    <t>7.97</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21},
+             {'volume': 200, 't_s':  10, 't':  50, 'A': 5, 'B': 26},
+             {'volume': 300, 't_s':  0, 't':  50, 'A': 4, 'B': 3},
+             {'volume': 100, 't_s':  100, 't':  50, 'A': 9, 'B': 17},
+             {'volume': 200, 't_s':  0, 't':  20, 'A': 12, 'B': 19},
+             {'volume': 100, 't_s':  50, 't':  50, 'A': 8, 'B': 5}]</t>
+  </si>
+  <si>
+    <t>13.66</t>
+  </si>
+  <si>
+    <t>7.36</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21},
+             {'volume': 200, 't_s':  10, 't':  50, 'A': 5, 'B': 26},
+             {'volume': 300, 't_s':  0, 't':  50, 'A': 4, 'B': 3},
+             {'volume': 100, 't_s':  100, 't':  50, 'A': 9, 'B': 17},
+             {'volume': 200, 't_s':  0, 't':  20, 'A': 12, 'B': 19},
+             {'volume': 100, 't_s':  50, 't':  50, 'A': 8, 'B': 5},
+             {'volume': 100, 't_s':  70, 't':  50, 'A': 26, 'B': 8}]</t>
+  </si>
+  <si>
+    <t>14.46</t>
+  </si>
+  <si>
+    <t>9.53</t>
+  </si>
+  <si>
+    <t>[{'volume': 900, 't_s':  60, 't':  60, 'A': 3, 'B': 8},
+             {'volume': 100, 't_s':  20, 't':  50, 'A': 7, 'B': 21},
+             {'volume': 200, 't_s':  10, 't':  50, 'A': 5, 'B': 26},
+             {'volume': 300, 't_s':  0, 't':  50, 'A': 4, 'B': 3},
+             {'volume': 100, 't_s':  100, 't':  50, 'A': 9, 'B': 17},
+             {'volume': 200, 't_s':  0, 't':  20, 'A': 12, 'B': 19},
+             {'volume': 100, 't_s':  50, 't':  50, 'A': 8, 'B': 5},
+             {'volume': 100, 't_s':  70, 't':  50, 'A': 26, 'B': 8},
+             {'volume': 100, 't_s':  40, 't':  50, 'A': 6, 'B': 30}]</t>
+  </si>
+  <si>
+    <t>22.021</t>
+  </si>
+  <si>
+    <t>11.91</t>
+  </si>
+  <si>
+    <t>27.35</t>
+  </si>
+  <si>
+    <t>15.27</t>
   </si>
 </sst>
 </file>
@@ -278,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -292,6 +410,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -310,6 +431,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -821,7 +946,7 @@
       <c r="D2" s="4">
         <v>2.0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -844,7 +969,7 @@
       <c r="D3" s="4">
         <v>3.0</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -867,7 +992,7 @@
       <c r="D4" s="4">
         <v>2.0</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -890,7 +1015,7 @@
       <c r="D5" s="4">
         <v>3.0</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -913,7 +1038,7 @@
       <c r="D6" s="4">
         <v>2.0</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -936,7 +1061,7 @@
       <c r="D7" s="4">
         <v>3.0</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -959,13 +1084,13 @@
       <c r="D8" s="4">
         <v>2.0</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -982,7 +1107,7 @@
       <c r="D9" s="4">
         <v>3.0</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1005,13 +1130,13 @@
       <c r="D10" s="4">
         <v>2.0</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1028,7 +1153,7 @@
       <c r="D11" s="4">
         <v>3.0</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>69</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1037,6 +1162,505 @@
       <c r="G11" s="4" t="s">
         <v>71</v>
       </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="6">
+        <v>43.0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="6">
+        <v>170.0</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="6">
+        <v>215.0</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="6">
+        <v>281.0</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="6">
+        <v>361.0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="6">
+        <v>404.0</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>9.0</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="6">
+        <v>519.0</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
+        <v>37.0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="6">
+        <v>632.0</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4">
+        <v>92.0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>96.0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4">
+        <v>92.0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>96.0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="6">
+        <v>92.0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>96.0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="6">
+        <v>92.0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>96.0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="6">
+        <v>158.0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>189.0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="6">
+        <v>158.0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>189.0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="6">
+        <v>737.0</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="6">
+        <v>158.0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>189.0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6">
+        <v>158.0</v>
+      </c>
+      <c r="C18" s="6">
+        <v>189.0</v>
+      </c>
+      <c r="D18" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="6">
+        <v>197.0</v>
+      </c>
+      <c r="C19" s="6">
+        <v>243.0</v>
+      </c>
+      <c r="D19" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6">
+        <v>197.0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>243.0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>197.0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>243.0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>197.0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>243.0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="F22" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>